<commit_message>
Enhancement to the Download Bill feature and README adjustments
</commit_message>
<xml_diff>
--- a/excel_tables/tables-with-the-apportionment-values/apportionment-values.xlsx
+++ b/excel_tables/tables-with-the-apportionment-values/apportionment-values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ecopredial\OneDrive\Área de Trabalho\refatorando\cajupe-bot-refatorado\excel_tables\tables-with-the-apportionment-values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44C9042-72DC-48E8-85A6-A97AE0D1BC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE6E18C-5668-42FE-886C-C1317771F35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{A5154430-D536-4265-BE1F-12977B4168E7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A5154430-D536-4265-BE1F-12977B4168E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>